<commit_message>
Added Database files + Fruit Scroll View with Linear layout
</commit_message>
<xml_diff>
--- a/DataBase/Diet_Data.xlsx
+++ b/DataBase/Diet_Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Fruits" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="152">
   <si>
     <t xml:space="preserve">Code</t>
   </si>
@@ -395,19 +395,91 @@
     <t xml:space="preserve">Paneer</t>
   </si>
   <si>
+    <t xml:space="preserve">Buttermilk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lassi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chicken</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP02</t>
+  </si>
+  <si>
     <t xml:space="preserve">Egg</t>
   </si>
   <si>
-    <t xml:space="preserve">Chicken</t>
+    <t xml:space="preserve">DP03</t>
   </si>
   <si>
     <t xml:space="preserve">Fish – fresh</t>
   </si>
   <si>
+    <t xml:space="preserve">DP04</t>
+  </si>
+  <si>
     <t xml:space="preserve">Fish – sea</t>
   </si>
   <si>
+    <t xml:space="preserve">DP05</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mutton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pork</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prawn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peanut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Walnut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pistachio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Masoor Dal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toor Dal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chikpeas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kidney Bean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Almond</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cashew</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moong Dal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arhar Dal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chana Dal</t>
   </si>
 </sst>
 </file>
@@ -510,7 +582,7 @@
   </sheetPr>
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -1050,10 +1122,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1103,6 +1175,16 @@
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
         <v>122</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1121,10 +1203,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1147,28 +1229,59 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>125</v>
+      </c>
       <c r="B2" s="0" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>127</v>
+      </c>
       <c r="B3" s="0" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>129</v>
+      </c>
       <c r="B4" s="0" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>131</v>
+      </c>
       <c r="B5" s="0" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>133</v>
+      </c>
       <c r="B6" s="0" t="s">
-        <v>127</v>
+        <v>134</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -1187,10 +1300,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1212,6 +1325,76 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="0" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="0" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="0" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="0" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="0" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="0" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="0" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="0" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0" t="s">
+        <v>151</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>